<commit_message>
added field as example to verify nominator knows nominee. made sure various elements are required.
</commit_message>
<xml_diff>
--- a/nominate_ambassadors.xlsx
+++ b/nominate_ambassadors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakehughey/Library/CloudStorage/GoogleDrive-jakejhughey@gmail.com/My Drive/career/suvita_ambassador_nominations/v04_stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakehughey/Library/CloudStorage/GoogleDrive-jakejhughey@gmail.com/My Drive/career/suvita/suvita-surveycto-ambassadors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95133F58-16C7-9A49-8DD5-53F7E6735323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B4E1C-70D7-6541-8C0E-593D8D0E472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="500" windowWidth="23900" windowHeight="21900" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="428">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2588,9 +2588,6 @@
     <t>select_one yesno</t>
   </si>
   <si>
-    <t>if(${nominee_new}=1 or ${update_phone}=1, ${nominee_phone_new}, pulldata('nominees', 'nominee_phone', 'nominee_key', ${nominee_key}))</t>
-  </si>
-  <si>
     <t>concat(${nominee_name}, ' - ', if(${nominee_phone} = -1, 'Phone number unknown', ${nominee_phone}))</t>
   </si>
   <si>
@@ -2661,6 +2658,18 @@
   </si>
   <si>
     <t>nominate_ambassadors</t>
+  </si>
+  <si>
+    <t>if(${nominee_new} = 1 or ${update_phone} = 1, ${nominee_phone_new}, pulldata('nominees', 'nominee_phone', 'nominee_key', ${nominee_key}))</t>
+  </si>
+  <si>
+    <t>nominee_age</t>
+  </si>
+  <si>
+    <t>Enter ${nominee_name}'s approximate age in years.</t>
+  </si>
+  <si>
+    <t>. &gt;= 18 and . &lt;= 110</t>
   </si>
 </sst>
 </file>
@@ -5202,11 +5211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5458,7 +5467,7 @@
       </c>
       <c r="D13" s="11"/>
       <c r="G13" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>392</v>
@@ -5540,74 +5549,86 @@
       </c>
       <c r="D18" s="11"/>
       <c r="N18" s="79" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>45</v>
+        <v>399</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>370</v>
+        <v>398</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>401</v>
       </c>
       <c r="D19" s="11"/>
-      <c r="N19" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="K19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="79"/>
+    </row>
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>399</v>
+        <v>43</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="D20" s="11"/>
       <c r="I20" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="G21" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>419</v>
-      </c>
-      <c r="N20" s="79"/>
-    </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="I21" s="9" t="s">
-        <v>421</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>378</v>
+        <v>425</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="D22" s="11"/>
       <c r="G22" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>420</v>
+        <v>427</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -5615,11 +5636,11 @@
         <v>45</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D23" s="11"/>
       <c r="N23" s="9" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -5627,33 +5648,33 @@
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="D24" s="11"/>
       <c r="N24" s="9" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>141</v>
+        <v>45</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="D25" s="11"/>
+      <c r="N25" s="9" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="D26" s="11"/>
-      <c r="N26" s="9" t="s">
-        <v>409</v>
-      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
@@ -5664,7 +5685,7 @@
       </c>
       <c r="D27" s="11"/>
       <c r="N27" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -5672,7 +5693,7 @@
         <v>45</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D28" s="11"/>
       <c r="N28" s="9" t="s">
@@ -5684,47 +5705,47 @@
         <v>45</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D29" s="11"/>
       <c r="N29" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="N30" s="9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="80" t="s">
+        <v>414</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="80" t="s">
-        <v>415</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="M30" s="9" t="s">
+      <c r="M31" s="9" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="N31" s="9">
-        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -5732,38 +5753,50 @@
         <v>45</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D32" s="11"/>
       <c r="N32" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="N33" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+    <row r="34" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B34" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C34" s="22" t="s">
         <v>374</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D34" s="11"/>
-      <c r="W34" s="9"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D35" s="11"/>
+      <c r="W35" s="9"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -6208,14 +6241,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2304181937</v>
+        <v>2304201559</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>

</xml_diff>